<commit_message>
cambio de algunos códigos
cambio de algunos códigos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion13/SolicitudGrafica_CN_07_13_CO_REC220 (NUEVO).xlsx
+++ b/fuentes/contenidos/grado07/guion13/SolicitudGrafica_CN_07_13_CO_REC220 (NUEVO).xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\Aulaplaneta All\Trabajos de editor\EDITOR\ESCALETAS\Escaletas  grupo  2\CN_07_13_CO Las ciencias al servicio de la Medicina\Recursos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
+    <workbookView xWindow="6980" yWindow="2300" windowWidth="27760" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -21,12 +16,17 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="193">
   <si>
     <t>Fecha:</t>
   </si>
@@ -597,9 +597,6 @@
   </si>
   <si>
     <t>CN_07_13_CO_REC220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://indipacklogistica.com/project/vinipel/#prettyPhoto[this_page]/0/ </t>
   </si>
   <si>
     <t>Ilustración</t>
@@ -618,7 +615,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -759,6 +756,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1011,11 +1013,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1024,7 +1026,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1032,17 +1034,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1052,7 +1054,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1060,12 +1062,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1074,18 +1076,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1115,11 +1117,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1129,10 +1131,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1142,7 +1144,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -1216,16 +1218,16 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1233,23 +1235,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1307,7 +1309,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1611,6 +1613,7 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1739,15 +1742,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:colOff>1041400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1760,7 +1763,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1768,20 +1771,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1794,15 +1783,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:colOff>1054100</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>866775</xdr:colOff>
+          <xdr:colOff>863600</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1815,7 +1804,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1823,20 +1812,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1849,15 +1824,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1870,7 +1845,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1878,20 +1853,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1906,13 +1867,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1925,7 +1886,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1933,20 +1894,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1959,15 +1906,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
+          <xdr:colOff>825500</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1980,7 +1927,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1988,20 +1935,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2014,15 +1947,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2035,7 +1968,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2043,20 +1976,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2069,15 +1988,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2090,7 +2009,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2098,20 +2017,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2444,33 +2349,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="71" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="34.83203125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="15" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.875" style="2"/>
+    <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2489,7 +2394,7 @@
         <v>Ubicación de la imagen en el recurso F13B</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>121</v>
@@ -2516,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2543,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="16.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
@@ -2571,7 +2476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="17.25" thickBot="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2600,7 +2505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2620,7 +2525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="30.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
         <v>40</v>
@@ -2645,7 +2550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.5" thickBot="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2669,7 +2574,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="38.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="38.75" customHeight="1" thickBot="1">
       <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
@@ -2705,7 +2610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="32.25" customHeight="1">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
@@ -2742,13 +2647,13 @@
       <c r="J10" s="62"/>
       <c r="K10" s="64"/>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="31.5" customHeight="1">
       <c r="A11" s="12" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="62">
-        <v>16336079</v>
+      <c r="B11" s="104">
+        <v>163336079</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2779,13 +2684,13 @@
       <c r="J11" s="62"/>
       <c r="K11" s="65"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="62">
-        <v>16336079</v>
+      <c r="B12" s="104">
+        <v>163336079</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2816,13 +2721,13 @@
       <c r="J12" s="62"/>
       <c r="K12" s="64"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="26.25" customHeight="1">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="62" t="s">
-        <v>190</v>
+      <c r="B13" s="104">
+        <v>209377015</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2853,7 +2758,7 @@
       <c r="J13" s="62"/>
       <c r="K13" s="64"/>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
@@ -2890,7 +2795,7 @@
       <c r="J14" s="62"/>
       <c r="K14" s="64"/>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="18.75" customHeight="1">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
@@ -2927,20 +2832,20 @@
       <c r="J15" s="62"/>
       <c r="K15" s="66"/>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F13B</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E16" s="63" t="s">
         <v>171</v>
@@ -2962,26 +2867,26 @@
         <v/>
       </c>
       <c r="J16" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="K16" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="K16" s="62" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" s="11" customFormat="1" ht="22.5" customHeight="1">
       <c r="A17" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F13B</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E17" s="63" t="s">
         <v>171</v>
@@ -3003,26 +2908,26 @@
         <v/>
       </c>
       <c r="J17" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="K17" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="K17" s="62" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" s="11" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG09</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F13B</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E18" s="63" t="s">
         <v>171</v>
@@ -3044,26 +2949,26 @@
         <v/>
       </c>
       <c r="J18" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="K18" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="K18" s="62" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F13B</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E19" s="63" t="s">
         <v>171</v>
@@ -3085,26 +2990,26 @@
         <v/>
       </c>
       <c r="J19" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="K19" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="K19" s="62" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="A20" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG11</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F13B</v>
       </c>
       <c r="D20" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E20" s="63" t="s">
         <v>171</v>
@@ -3126,26 +3031,26 @@
         <v/>
       </c>
       <c r="J20" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="K20" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="K20" s="62" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" s="11" customFormat="1" ht="17.25" customHeight="1">
       <c r="A21" s="12" t="str">
         <f t="shared" si="6"/>
         <v>IMG12</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F13B</v>
       </c>
       <c r="D21" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E21" s="63" t="s">
         <v>171</v>
@@ -3167,13 +3072,13 @@
         <v/>
       </c>
       <c r="J21" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="K21" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="K21" s="62" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A22" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3204,7 +3109,7 @@
       <c r="J22" s="63"/>
       <c r="K22" s="67"/>
     </row>
-    <row r="23" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A23" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3235,7 +3140,7 @@
       <c r="J23" s="64"/>
       <c r="K23" s="64"/>
     </row>
-    <row r="24" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A24" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3266,7 +3171,7 @@
       <c r="J24" s="63"/>
       <c r="K24" s="65"/>
     </row>
-    <row r="25" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A25" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3297,7 +3202,7 @@
       <c r="J25" s="63"/>
       <c r="K25" s="64"/>
     </row>
-    <row r="26" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A26" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3328,7 +3233,7 @@
       <c r="J26" s="63"/>
       <c r="K26" s="64"/>
     </row>
-    <row r="27" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A27" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3359,7 +3264,7 @@
       <c r="J27" s="64"/>
       <c r="K27" s="64"/>
     </row>
-    <row r="28" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A28" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3390,7 +3295,7 @@
       <c r="J28" s="64"/>
       <c r="K28" s="64"/>
     </row>
-    <row r="29" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A29" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3421,7 +3326,7 @@
       <c r="J29" s="64"/>
       <c r="K29" s="64"/>
     </row>
-    <row r="30" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A30" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3452,7 +3357,7 @@
       <c r="J30" s="64"/>
       <c r="K30" s="64"/>
     </row>
-    <row r="31" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A31" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3483,7 +3388,7 @@
       <c r="J31" s="64"/>
       <c r="K31" s="64"/>
     </row>
-    <row r="32" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A32" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3514,7 +3419,7 @@
       <c r="J32" s="64"/>
       <c r="K32" s="64"/>
     </row>
-    <row r="33" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A33" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3545,7 +3450,7 @@
       <c r="J33" s="64"/>
       <c r="K33" s="64"/>
     </row>
-    <row r="34" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A34" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3576,7 +3481,7 @@
       <c r="J34" s="64"/>
       <c r="K34" s="64"/>
     </row>
-    <row r="35" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A35" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3607,7 +3512,7 @@
       <c r="J35" s="63"/>
       <c r="K35" s="65"/>
     </row>
-    <row r="36" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A36" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3638,7 +3543,7 @@
       <c r="J36" s="63"/>
       <c r="K36" s="65"/>
     </row>
-    <row r="37" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A37" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3669,7 +3574,7 @@
       <c r="J37" s="68"/>
       <c r="K37" s="65"/>
     </row>
-    <row r="38" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A38" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3700,7 +3605,7 @@
       <c r="J38" s="69"/>
       <c r="K38" s="65"/>
     </row>
-    <row r="39" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A39" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3731,7 +3636,7 @@
       <c r="J39" s="63"/>
       <c r="K39" s="65"/>
     </row>
-    <row r="40" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A40" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3762,7 +3667,7 @@
       <c r="J40" s="63"/>
       <c r="K40" s="65"/>
     </row>
-    <row r="41" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A41" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3793,7 +3698,7 @@
       <c r="J41" s="63"/>
       <c r="K41" s="65"/>
     </row>
-    <row r="42" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A42" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3824,7 +3729,7 @@
       <c r="J42" s="63"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A43" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3855,7 +3760,7 @@
       <c r="J43" s="63"/>
       <c r="K43" s="65"/>
     </row>
-    <row r="44" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A44" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3886,7 +3791,7 @@
       <c r="J44" s="63"/>
       <c r="K44" s="65"/>
     </row>
-    <row r="45" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A45" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3917,7 +3822,7 @@
       <c r="J45" s="63"/>
       <c r="K45" s="65"/>
     </row>
-    <row r="46" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A46" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3948,7 +3853,7 @@
       <c r="J46" s="63"/>
       <c r="K46" s="65"/>
     </row>
-    <row r="47" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A47" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3979,7 +3884,7 @@
       <c r="J47" s="63"/>
       <c r="K47" s="65"/>
     </row>
-    <row r="48" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A48" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4010,7 +3915,7 @@
       <c r="J48" s="63"/>
       <c r="K48" s="65"/>
     </row>
-    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A49" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4041,7 +3946,7 @@
       <c r="J49" s="63"/>
       <c r="K49" s="65"/>
     </row>
-    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A50" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4072,7 +3977,7 @@
       <c r="J50" s="63"/>
       <c r="K50" s="65"/>
     </row>
-    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A51" s="12" t="str">
         <f t="shared" ref="A51:A82" si="8">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
         <v/>
@@ -4103,7 +4008,7 @@
       <c r="J51" s="63"/>
       <c r="K51" s="65"/>
     </row>
-    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A52" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4134,7 +4039,7 @@
       <c r="J52" s="63"/>
       <c r="K52" s="65"/>
     </row>
-    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A53" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4165,7 +4070,7 @@
       <c r="J53" s="63"/>
       <c r="K53" s="65"/>
     </row>
-    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A54" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4196,7 +4101,7 @@
       <c r="J54" s="63"/>
       <c r="K54" s="65"/>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A55" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4227,7 +4132,7 @@
       <c r="J55" s="63"/>
       <c r="K55" s="65"/>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A56" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4258,7 +4163,7 @@
       <c r="J56" s="63"/>
       <c r="K56" s="65"/>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A57" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4289,7 +4194,7 @@
       <c r="J57" s="63"/>
       <c r="K57" s="65"/>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A58" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4320,7 +4225,7 @@
       <c r="J58" s="63"/>
       <c r="K58" s="65"/>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A59" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4351,7 +4256,7 @@
       <c r="J59" s="63"/>
       <c r="K59" s="65"/>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A60" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4382,7 +4287,7 @@
       <c r="J60" s="63"/>
       <c r="K60" s="65"/>
     </row>
-    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A61" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4413,7 +4318,7 @@
       <c r="J61" s="63"/>
       <c r="K61" s="65"/>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A62" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4444,7 +4349,7 @@
       <c r="J62" s="63"/>
       <c r="K62" s="65"/>
     </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A63" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4475,7 +4380,7 @@
       <c r="J63" s="63"/>
       <c r="K63" s="65"/>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A64" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4506,7 +4411,7 @@
       <c r="J64" s="63"/>
       <c r="K64" s="65"/>
     </row>
-    <row r="65" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A65" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4537,7 +4442,7 @@
       <c r="J65" s="63"/>
       <c r="K65" s="65"/>
     </row>
-    <row r="66" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A66" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4568,7 +4473,7 @@
       <c r="J66" s="63"/>
       <c r="K66" s="65"/>
     </row>
-    <row r="67" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A67" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4599,7 +4504,7 @@
       <c r="J67" s="63"/>
       <c r="K67" s="65"/>
     </row>
-    <row r="68" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A68" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4630,7 +4535,7 @@
       <c r="J68" s="63"/>
       <c r="K68" s="65"/>
     </row>
-    <row r="69" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A69" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4661,7 +4566,7 @@
       <c r="J69" s="63"/>
       <c r="K69" s="65"/>
     </row>
-    <row r="70" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A70" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4692,7 +4597,7 @@
       <c r="J70" s="63"/>
       <c r="K70" s="65"/>
     </row>
-    <row r="71" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A71" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4723,7 +4628,7 @@
       <c r="J71" s="63"/>
       <c r="K71" s="65"/>
     </row>
-    <row r="72" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A72" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4754,7 +4659,7 @@
       <c r="J72" s="63"/>
       <c r="K72" s="65"/>
     </row>
-    <row r="73" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A73" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4785,7 +4690,7 @@
       <c r="J73" s="63"/>
       <c r="K73" s="65"/>
     </row>
-    <row r="74" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A74" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4816,7 +4721,7 @@
       <c r="J74" s="63"/>
       <c r="K74" s="65"/>
     </row>
-    <row r="75" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A75" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4847,7 +4752,7 @@
       <c r="J75" s="63"/>
       <c r="K75" s="65"/>
     </row>
-    <row r="76" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A76" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4878,7 +4783,7 @@
       <c r="J76" s="63"/>
       <c r="K76" s="65"/>
     </row>
-    <row r="77" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A77" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4909,7 +4814,7 @@
       <c r="J77" s="63"/>
       <c r="K77" s="65"/>
     </row>
-    <row r="78" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A78" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4940,7 +4845,7 @@
       <c r="J78" s="63"/>
       <c r="K78" s="65"/>
     </row>
-    <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A79" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4971,7 +4876,7 @@
       <c r="J79" s="63"/>
       <c r="K79" s="65"/>
     </row>
-    <row r="80" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A80" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5002,7 +4907,7 @@
       <c r="J80" s="63"/>
       <c r="K80" s="65"/>
     </row>
-    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A81" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5033,7 +4938,7 @@
       <c r="J81" s="63"/>
       <c r="K81" s="65"/>
     </row>
-    <row r="82" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A82" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5064,7 +4969,7 @@
       <c r="J82" s="63"/>
       <c r="K82" s="65"/>
     </row>
-    <row r="83" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A83" s="12" t="str">
         <f t="shared" ref="A83:A108" si="12">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
         <v/>
@@ -5095,7 +5000,7 @@
       <c r="J83" s="63"/>
       <c r="K83" s="65"/>
     </row>
-    <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A84" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5126,7 +5031,7 @@
       <c r="J84" s="63"/>
       <c r="K84" s="65"/>
     </row>
-    <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A85" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5157,7 +5062,7 @@
       <c r="J85" s="63"/>
       <c r="K85" s="65"/>
     </row>
-    <row r="86" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A86" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5188,7 +5093,7 @@
       <c r="J86" s="63"/>
       <c r="K86" s="65"/>
     </row>
-    <row r="87" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A87" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5219,7 +5124,7 @@
       <c r="J87" s="63"/>
       <c r="K87" s="65"/>
     </row>
-    <row r="88" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A88" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5250,7 +5155,7 @@
       <c r="J88" s="63"/>
       <c r="K88" s="65"/>
     </row>
-    <row r="89" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A89" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5281,7 +5186,7 @@
       <c r="J89" s="63"/>
       <c r="K89" s="65"/>
     </row>
-    <row r="90" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A90" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5312,7 +5217,7 @@
       <c r="J90" s="63"/>
       <c r="K90" s="65"/>
     </row>
-    <row r="91" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A91" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5343,7 +5248,7 @@
       <c r="J91" s="63"/>
       <c r="K91" s="65"/>
     </row>
-    <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A92" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5374,7 +5279,7 @@
       <c r="J92" s="63"/>
       <c r="K92" s="65"/>
     </row>
-    <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A93" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5405,7 +5310,7 @@
       <c r="J93" s="63"/>
       <c r="K93" s="65"/>
     </row>
-    <row r="94" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A94" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5436,7 +5341,7 @@
       <c r="J94" s="63"/>
       <c r="K94" s="65"/>
     </row>
-    <row r="95" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A95" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5467,7 +5372,7 @@
       <c r="J95" s="63"/>
       <c r="K95" s="65"/>
     </row>
-    <row r="96" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A96" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5498,7 +5403,7 @@
       <c r="J96" s="63"/>
       <c r="K96" s="65"/>
     </row>
-    <row r="97" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A97" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5529,7 +5434,7 @@
       <c r="J97" s="63"/>
       <c r="K97" s="65"/>
     </row>
-    <row r="98" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A98" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5560,7 +5465,7 @@
       <c r="J98" s="63"/>
       <c r="K98" s="65"/>
     </row>
-    <row r="99" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A99" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5591,7 +5496,7 @@
       <c r="J99" s="63"/>
       <c r="K99" s="65"/>
     </row>
-    <row r="100" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A100" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5622,7 +5527,7 @@
       <c r="J100" s="63"/>
       <c r="K100" s="65"/>
     </row>
-    <row r="101" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A101" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5653,7 +5558,7 @@
       <c r="J101" s="63"/>
       <c r="K101" s="65"/>
     </row>
-    <row r="102" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A102" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5684,7 +5589,7 @@
       <c r="J102" s="63"/>
       <c r="K102" s="65"/>
     </row>
-    <row r="103" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A103" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5715,7 +5620,7 @@
       <c r="J103" s="63"/>
       <c r="K103" s="65"/>
     </row>
-    <row r="104" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A104" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5746,7 +5651,7 @@
       <c r="J104" s="63"/>
       <c r="K104" s="65"/>
     </row>
-    <row r="105" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A105" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5777,7 +5682,7 @@
       <c r="J105" s="63"/>
       <c r="K105" s="65"/>
     </row>
-    <row r="106" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A106" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5808,7 +5713,7 @@
       <c r="J106" s="63"/>
       <c r="K106" s="65"/>
     </row>
-    <row r="107" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A107" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5839,7 +5744,7 @@
       <c r="J107" s="63"/>
       <c r="K107" s="65"/>
     </row>
-    <row r="108" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A108" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5911,31 +5816,36 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
+  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="22" customWidth="1"/>
-    <col min="2" max="2" width="11" style="22"/>
-    <col min="3" max="3" width="13.875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="22" customWidth="1"/>
-    <col min="5" max="7" width="11" style="22"/>
+    <col min="1" max="1" width="72.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="22"/>
+    <col min="3" max="3" width="13.83203125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="22" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="22"/>
     <col min="8" max="11" width="11" style="22" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="22"/>
+    <col min="12" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1">
       <c r="A1" s="88" t="s">
         <v>38</v>
       </c>
@@ -5945,7 +5855,7 @@
       <c r="E1" s="89"/>
       <c r="F1" s="90"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
@@ -5957,7 +5867,7 @@
       <c r="E2" s="93"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="63">
       <c r="A3" s="33" t="s">
         <v>43</v>
       </c>
@@ -5981,7 +5891,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.5">
       <c r="A4" s="30" t="s">
         <v>44</v>
       </c>
@@ -6009,7 +5919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1">
       <c r="A5" s="33" t="s">
         <v>45</v>
       </c>
@@ -6036,7 +5946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -6058,7 +5968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="48" thickBot="1">
       <c r="A7" s="33" t="s">
         <v>11</v>
       </c>
@@ -6085,7 +5995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="47.25">
       <c r="A8" s="33" t="s">
         <v>53</v>
       </c>
@@ -6104,7 +6014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="47.25">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -6123,7 +6033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1">
       <c r="A10" s="34" t="s">
         <v>36</v>
       </c>
@@ -6142,7 +6052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="I11" s="22" t="s">
         <v>32</v>
       </c>
@@ -6153,7 +6063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1">
       <c r="I12" s="22" t="s">
         <v>37</v>
       </c>
@@ -6164,7 +6074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="88" t="s">
         <v>41</v>
       </c>
@@ -6183,7 +6093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1">
       <c r="A14" s="33"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -6200,7 +6110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="30" t="s">
         <v>46</v>
       </c>
@@ -6218,7 +6128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="67.25" customHeight="1">
       <c r="A16" s="33" t="s">
         <v>47</v>
       </c>
@@ -6242,7 +6152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="32" customHeight="1" thickBot="1">
       <c r="A17" s="30" t="s">
         <v>44</v>
       </c>
@@ -6263,7 +6173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1">
       <c r="A18" s="33" t="s">
         <v>48</v>
       </c>
@@ -6284,7 +6194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
@@ -6303,7 +6213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1">
       <c r="A20" s="34" t="s">
         <v>51</v>
       </c>
@@ -6325,7 +6235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="H21" s="22" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -6342,122 +6252,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="K22" s="22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="K23" s="22">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="K24" s="22">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="K25" s="22">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="K26" s="22">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="K27" s="22">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="K28" s="22">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="K29" s="22">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="K30" s="22">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="K31" s="22">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="K32" s="22">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11">
       <c r="K33" s="22">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11">
       <c r="K34" s="22">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11">
       <c r="K35" s="22">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11">
       <c r="K36" s="22">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11">
       <c r="K37" s="22">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11">
       <c r="K38" s="22">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11">
       <c r="K39" s="22">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11">
       <c r="K40" s="22">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:11">
       <c r="K41" s="22">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="11:11">
       <c r="K42" s="22">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="11:11">
       <c r="K43" s="22">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="11:11">
       <c r="K44" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="11:11">
       <c r="K45" s="22" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6476,169 +6386,182 @@
     <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId4" name="Drop Down 6">
+            <control shapeId="1030" r:id="rId3" name="Drop Down 6">
               <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId5" name="Drop Down 7">
+            <control shapeId="1031" r:id="rId4" name="Drop Down 7">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>828675</xdr:colOff>
+                    <xdr:colOff>825500</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId6" name="Drop Down 8">
+            <control shapeId="1032" r:id="rId5" name="Drop Down 8">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId7" name="Drop Down 11">
+            <control shapeId="1035" r:id="rId6" name="Drop Down 11">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId8" name="Drop Down 2">
+            <control shapeId="1026" r:id="rId7" name="Drop Down 2">
               <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:colOff>1041400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId9" name="Drop Down 4">
+            <control shapeId="1028" r:id="rId8" name="Drop Down 4">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:colOff>1054100</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>866775</xdr:colOff>
+                    <xdr:colOff>863600</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId10" name="Drop Down 5">
+            <control shapeId="1029" r:id="rId9" name="Drop Down 5">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6651,22 +6574,22 @@
       <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="22" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="22" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="22" customWidth="1"/>
     <col min="3" max="3" width="17" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.75" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.875" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.75" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="22" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="22" customWidth="1"/>
-    <col min="9" max="9" width="27.25" style="22" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" style="22" customWidth="1"/>
     <col min="10" max="10" width="44.5" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="22"/>
+    <col min="11" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="103" t="s">
         <v>56</v>
       </c>
@@ -6693,7 +6616,7 @@
       </c>
       <c r="I1" s="102"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="103"/>
       <c r="B2" s="103"/>
       <c r="C2" s="103"/>
@@ -6708,7 +6631,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
@@ -6733,7 +6656,7 @@
       </c>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A4" s="42" t="s">
         <v>57</v>
       </c>
@@ -6762,7 +6685,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A5" s="43" t="s">
         <v>77</v>
       </c>
@@ -6791,7 +6714,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A6" s="42" t="s">
         <v>58</v>
       </c>
@@ -6820,7 +6743,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A7" s="42" t="s">
         <v>58</v>
       </c>
@@ -6845,7 +6768,7 @@
       </c>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A8" s="42" t="s">
         <v>80</v>
       </c>
@@ -6874,7 +6797,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A9" s="42" t="s">
         <v>82</v>
       </c>
@@ -6903,7 +6826,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A10" s="42" t="s">
         <v>84</v>
       </c>
@@ -6932,7 +6855,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A11" s="42" t="s">
         <v>86</v>
       </c>
@@ -6957,7 +6880,7 @@
       </c>
       <c r="I11" s="42"/>
     </row>
-    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
@@ -6986,7 +6909,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A13" s="42" t="s">
         <v>91</v>
       </c>
@@ -7015,7 +6938,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="14.75" customHeight="1">
       <c r="A14" s="44" t="s">
         <v>94</v>
       </c>
@@ -7038,7 +6961,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="14.75" customHeight="1">
       <c r="A15" s="44" t="s">
         <v>96</v>
       </c>
@@ -7064,7 +6987,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="14.75" customHeight="1">
       <c r="A16" s="46" t="s">
         <v>100</v>
       </c>
@@ -7092,7 +7015,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="14.75" customHeight="1">
       <c r="A17" s="42" t="s">
         <v>103</v>
       </c>
@@ -7120,7 +7043,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="14.75" customHeight="1">
       <c r="A18" s="42" t="s">
         <v>149</v>
       </c>
@@ -7146,7 +7069,7 @@
       <c r="I18" s="44"/>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="14.75" customHeight="1">
       <c r="A19" s="42" t="s">
         <v>137</v>
       </c>
@@ -7170,7 +7093,7 @@
       <c r="I19" s="44"/>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="14.75" customHeight="1">
       <c r="A20" s="42" t="s">
         <v>137</v>
       </c>
@@ -7194,7 +7117,7 @@
       <c r="I20" s="44"/>
       <c r="J20" s="49"/>
     </row>
-    <row r="21" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="14.75" customHeight="1">
       <c r="A21" s="42" t="s">
         <v>137</v>
       </c>
@@ -7218,7 +7141,7 @@
       <c r="I21" s="70"/>
       <c r="J21" s="49"/>
     </row>
-    <row r="22" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="14.75" customHeight="1">
       <c r="A22" s="44" t="s">
         <v>132</v>
       </c>
@@ -7242,7 +7165,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="14.75" customHeight="1">
       <c r="A23" s="42" t="s">
         <v>132</v>
       </c>
@@ -7271,7 +7194,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="14.75" customHeight="1">
       <c r="A24" s="42" t="s">
         <v>134</v>
       </c>
@@ -7286,7 +7209,7 @@
       <c r="H24" s="44"/>
       <c r="I24" s="44"/>
     </row>
-    <row r="25" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="14.75" customHeight="1">
       <c r="A25" s="42" t="s">
         <v>135</v>
       </c>
@@ -7310,7 +7233,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="14.75" customHeight="1">
       <c r="A26" s="42" t="s">
         <v>135</v>
       </c>
@@ -7339,7 +7262,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="14.75" customHeight="1">
       <c r="A27" s="42" t="s">
         <v>138</v>
       </c>
@@ -7363,7 +7286,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="14.75" customHeight="1">
       <c r="A28" s="42" t="s">
         <v>138</v>
       </c>
@@ -7387,7 +7310,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="14.75" customHeight="1">
       <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
@@ -7416,7 +7339,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="14.75" customHeight="1">
       <c r="A30" s="42" t="s">
         <v>139</v>
       </c>
@@ -7439,7 +7362,7 @@
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
     </row>
-    <row r="31" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="14.75" customHeight="1">
       <c r="A31" s="42" t="s">
         <v>140</v>
       </c>
@@ -7456,7 +7379,7 @@
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
     </row>
-    <row r="32" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="14.75" customHeight="1">
       <c r="A32" s="42" t="s">
         <v>141</v>
       </c>
@@ -7471,7 +7394,7 @@
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="14.75" customHeight="1">
       <c r="A33" s="42" t="s">
         <v>136</v>
       </c>
@@ -7488,7 +7411,7 @@
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="14.75" customHeight="1">
       <c r="A34" s="42" t="s">
         <v>142</v>
       </c>
@@ -7503,7 +7426,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
     </row>
-    <row r="35" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="14.75" customHeight="1">
       <c r="A35" s="42" t="s">
         <v>95</v>
       </c>
@@ -7532,7 +7455,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="14.75" customHeight="1">
       <c r="A36" s="42" t="s">
         <v>95</v>
       </c>
@@ -7561,7 +7484,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="14.75" customHeight="1">
       <c r="A37" s="42" t="s">
         <v>143</v>
       </c>
@@ -7584,7 +7507,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
     </row>
-    <row r="38" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="14.75" customHeight="1">
       <c r="A38" s="42" t="s">
         <v>143</v>
       </c>
@@ -7607,13 +7530,13 @@
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="50" t="s">
         <v>107</v>
       </c>
       <c r="B40" s="50"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="51" t="s">
         <v>108</v>
       </c>
@@ -7627,7 +7550,7 @@
       <c r="E41" s="52"/>
       <c r="F41" s="52"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="54" t="s">
         <v>109</v>
       </c>
@@ -7641,7 +7564,7 @@
       <c r="E42" s="55"/>
       <c r="F42" s="55"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="54" t="s">
         <v>110</v>
       </c>
@@ -7655,7 +7578,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="55"/>
     </row>
-    <row r="44" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="31.5">
       <c r="A44" s="54" t="s">
         <v>111</v>
       </c>
@@ -7669,7 +7592,7 @@
       <c r="E44" s="55"/>
       <c r="F44" s="55"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="54" t="s">
         <v>112</v>
       </c>
@@ -7683,7 +7606,7 @@
       <c r="E45" s="55"/>
       <c r="F45" s="55"/>
     </row>
-    <row r="46" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="47.25">
       <c r="A46" s="54" t="s">
         <v>164</v>
       </c>
@@ -7711,5 +7634,10 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>